<commit_message>
updated with optional cookie
</commit_message>
<xml_diff>
--- a/summary-info.xlsx
+++ b/summary-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/github/ms-fs-performance-testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E65D79-159B-2C4F-A476-71CC1B4E51AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B40F0F-2FB7-CC41-8FE2-1D0DA04479E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20860" yWindow="1080" windowWidth="35700" windowHeight="21240" activeTab="1" xr2:uid="{8E989FE0-EC17-C94D-8489-988F3A88D2B8}"/>
+    <workbookView xWindow="-32020" yWindow="-100" windowWidth="30800" windowHeight="16000" xr2:uid="{8E989FE0-EC17-C94D-8489-988F3A88D2B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="202">
   <si>
     <t># concurrent requests</t>
   </si>
@@ -499,12 +499,311 @@
   <si>
     <t>java -cp ./ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 http://10.244.0.35:9000/arcgis/rest/services/ safegraph 30 200 ./docs/safegraph2.txt 800 ./docs/output2_30a_200-2019-1107-fs.txt &gt; ./docs/standard_output2_30a_200-2019-1107-fs.txt</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">actor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">default-dispatcher = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">fork-join-executor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">parallelism-factor = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>6.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">parallelism-min = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">parallelism-max = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 10 200 ./docs_kube1/safegraph2.txt 200 ./docs_kube1/output2_fs_10_200-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_10_200-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 9 200 ./docs_kube1/safegraph2.txt 0 ./docs_kube1/output2</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 11 400 ./docs_kube1/safegraph2.txt 400 ./docs_kube1/output2_fs_11_200-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_11_200-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 12 200 ./docs_kube1/safegraph2.txt 600 ./docs_kube1/output2_fs_12_200-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_12_200-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 12 400 ./docs_kube1/safegraph2.txt 800 ./docs_kube1/output2_fs_12_400-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_12_400-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 12 600 ./docs_kube1/safegraph2.txt 1200 ./docs_kube1/output2_fs_12_600-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_12_600-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 200 ./docs_kube1/safegraph2.txt 1800 ./docs_kube1/output2_fs_13_300-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_13_200-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>From Laptop/evelope-set1</t>
+  </si>
+  <si>
+    <t>From Laptop/evelope-set2</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 600 ./docs_kube1/safegraph2.txt 2400 ./docs_kube1/output2_fs_13_600-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_13_600-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 400 ./docs_kube1/safegraph2.txt 2000 ./docs_kube1/output2_fs_13_400-2019-113.txt &gt; ./docs_kube1/standard-output2_fs_13_400-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 800 ./docs_kube1/safegraph1.txt 0 ./docs_kube1/output1_fs_13_800-2019-113.txt &gt; ./docs_kube1/standard-output1_fs_13_800-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 14 200 ./docs_kube1/safegraph1.txt 800 ./docs_kube1/output1_fs_14_400-2019-113.txt &gt; ./docs_kube1/standard-output1_fs_14_200-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 15 200 ./docs_kube1/safegraph1.txt 1000 ./docs_kube1/output1_fs_15_200-2019-113.txt &gt; ./docs_kube1/standard-output1_fs_15_200-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.FeatureServiceConcurrentTester1 https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 15 400 ./docs_kube1/safegraph1.txt 1200 ./docs_kube1/output1_fs_15_400-2019-113.txt &gt; ./docs_kube1/standard-output1_fs_15_400-2019-1113.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 10 200 ./docs_kube1/safegraph3.txt 0 ./docs_kube1/output3_10_200-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_10_200-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 11 200 ./docs_kube1/safegraph3.txt 200 ./docs_kube1/output3_11_200-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_11_200-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 12 200 ./docs_kube1/safegraph3.txt 200 ./docs_kube1/output3_12_200-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_12_200-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 12 200 ./docs_kube1/safegraph3.txt 400 ./docs_kube1/output3_12_200-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_12_200-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>3 -  datastore cached</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 12 600 ./docs_kube1/safegraph3.txt 600 ./docs_kube1/output3_12_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_12_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 200 ./docs_kube1/safegraph3.txt 1200 ./docs_kube1/output3_13_200-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_13_200-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 14 400 ./docs_kube1/safegraph3.txt 1800 ./docs_kube1/output3_14_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_14_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 400 ./docs_kube1/safegraph3.txt 1400 ./docs_kube1/output3_13_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_13_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 15 400 ./docs_kube1/safegraph3.txt 2200 ./docs_kube1/output3_15_500-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_15_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 16 400 ./docs_kube1/safegraph3.txt 2600 ./docs_kube1/output3_16_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output3_16_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 17 400 ./docs_kube1/safegraph1.txt 0 ./docs_kube1/output1_17_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_17_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 16 400 ./docs_kube1/safegraph1.txt 400 ./docs_kube1/output1_16_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_16_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>12 - Mat Crashed</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 16 300 ./docs_kube1/safegraph1.txt 800 ./docs_kube1/output1_16_300-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_16_300-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>13 - Mat crashed</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 15 300 ./docs_kube1/safegraph1.txt 1100 ./docs_kube1/output1_15_300-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_15_300-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>From Latop / envelope-set1, envelopes are biger than set3?</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 14 300 ./docs_kube1/safegraph1.txt 1400 ./docs_kube1/output1_14_300-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_14_300-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 300 ./docs_kube1/safegraph1.txt 1700 ./docs_kube1/output1_13_300-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_13_300-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 600 ./docs_kube1/safegraph1.txt 2400 ./docs_kube1/output1_13_600-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_13_600-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 400 ./docs_kube1/safegraph1.txt 2000 ./docs_kube1/output1_13_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output1_13_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>From Latop / envelope-set2</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 600 ./docs_kube1/safegraph2.txt 0 ./docs_kube1/output2_13_600-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_13_600-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 14 400 ./docs_kube1/safegraph2.txt 600 ./docs_kube1/output2_14_400-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_14_400-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>6 - Mat Crashed</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 22 100 ./docs_kube1/safegraph2.txt 1100 ./docs_kube1/output2_22_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_22_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 20 100 ./docs_kube1/safegraph2.txt 1000 ./docs_kube1/output2_20_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_20_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 30 100 ./docs_kube1/safegraph2.txt 1200 ./docs_kube1/output2_30_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_30_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 40 100 ./docs_kube1/safegraph2.txt 1300 ./docs_kube1/output2_40_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_40_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 100 100 ./docs_kube1/safegraph2.txt 1400 ./docs_kube1/output2_100_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_100_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 50 100 ./docs_kube1/safegraph2.txt 1500 ./docs_kube1/output2_50_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_50_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 100 ./docs_kube1/safegraph2.txt 1600 ./docs_kube1/output2_13_100-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_13_100-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>java -cp ./target/ms-fs-performance-test-1.0-jar-with-dependencies.jar com.esri.arcgis.performance.test.mat.MapServiceConcurrentTester https://us-iotdev.arcgis.com/fx1112a/7227004598d39e55/maps/arcgis/rest/services/ safegraph 13 1000 ./docs_kube1/safegraph2.txt 1700 ./docs_kube1/output2_13_1000-2019-1114-ms.txt flatHexagon &gt; ./docs_kube1/standard-output2_13_1000-2019-1114-ms.txt</t>
+  </si>
+  <si>
+    <t>5 - MAT crashed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -579,6 +878,26 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -606,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -624,6 +943,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26382,10 +26704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AE1DBA-CD56-294B-B978-A723FB34EE23}">
-  <dimension ref="A1:H415"/>
+  <dimension ref="A1:H480"/>
   <sheetViews>
-    <sheetView topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="G419" sqref="G419"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="B437" sqref="B437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30281,6 +30603,1046 @@
         <v>139</v>
       </c>
     </row>
+    <row r="419" spans="1:7" ht="19">
+      <c r="A419" s="17">
+        <v>43782</v>
+      </c>
+      <c r="B419" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7">
+      <c r="B420" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7">
+      <c r="B421" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7">
+      <c r="B422" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7">
+      <c r="B423" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7">
+      <c r="B424" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7">
+      <c r="B425" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7">
+      <c r="B426" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7">
+      <c r="B427" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7">
+      <c r="A428" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7">
+      <c r="A429">
+        <v>200</v>
+      </c>
+      <c r="B429">
+        <v>9</v>
+      </c>
+      <c r="C429">
+        <v>5938</v>
+      </c>
+      <c r="D429">
+        <v>0</v>
+      </c>
+      <c r="G429" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7">
+      <c r="A430">
+        <v>200</v>
+      </c>
+      <c r="B430">
+        <v>10</v>
+      </c>
+      <c r="C430">
+        <v>5979</v>
+      </c>
+      <c r="D430">
+        <v>0</v>
+      </c>
+      <c r="G430" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7">
+      <c r="A431">
+        <v>400</v>
+      </c>
+      <c r="B431">
+        <v>11</v>
+      </c>
+      <c r="C431">
+        <v>6747</v>
+      </c>
+      <c r="D431">
+        <v>0</v>
+      </c>
+      <c r="G431" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7">
+      <c r="A432">
+        <v>200</v>
+      </c>
+      <c r="B432">
+        <v>12</v>
+      </c>
+      <c r="C432">
+        <v>7524</v>
+      </c>
+      <c r="D432">
+        <v>0</v>
+      </c>
+      <c r="G432" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7">
+      <c r="A433">
+        <v>400</v>
+      </c>
+      <c r="B433">
+        <v>12</v>
+      </c>
+      <c r="C433">
+        <v>7772</v>
+      </c>
+      <c r="D433">
+        <v>0</v>
+      </c>
+      <c r="G433" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7">
+      <c r="A434">
+        <v>600</v>
+      </c>
+      <c r="B434">
+        <v>12</v>
+      </c>
+      <c r="C434">
+        <v>7377</v>
+      </c>
+      <c r="D434">
+        <v>0</v>
+      </c>
+      <c r="G434" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7">
+      <c r="A435">
+        <v>200</v>
+      </c>
+      <c r="B435">
+        <v>13</v>
+      </c>
+      <c r="C435">
+        <v>8656</v>
+      </c>
+      <c r="D435">
+        <f>3/200</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G435" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7">
+      <c r="A436">
+        <v>400</v>
+      </c>
+      <c r="B436">
+        <v>13</v>
+      </c>
+      <c r="C436">
+        <v>8262</v>
+      </c>
+      <c r="D436">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G436" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7">
+      <c r="A437">
+        <v>600</v>
+      </c>
+      <c r="B437">
+        <v>13</v>
+      </c>
+      <c r="C437">
+        <v>8366</v>
+      </c>
+      <c r="D437">
+        <f>2/400</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G437" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7">
+      <c r="A438" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7">
+      <c r="A439">
+        <v>800</v>
+      </c>
+      <c r="B439">
+        <v>13</v>
+      </c>
+      <c r="C439">
+        <v>8205</v>
+      </c>
+      <c r="D439">
+        <v>0</v>
+      </c>
+      <c r="G439" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7">
+      <c r="A440">
+        <v>200</v>
+      </c>
+      <c r="B440">
+        <v>14</v>
+      </c>
+      <c r="C440">
+        <v>9165</v>
+      </c>
+      <c r="D440">
+        <v>0</v>
+      </c>
+      <c r="G440" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7">
+      <c r="A441">
+        <v>200</v>
+      </c>
+      <c r="B441">
+        <v>15</v>
+      </c>
+      <c r="C441">
+        <v>9639</v>
+      </c>
+      <c r="D441">
+        <f>16/200</f>
+        <v>0.08</v>
+      </c>
+      <c r="G441" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7">
+      <c r="A442">
+        <v>400</v>
+      </c>
+      <c r="B442">
+        <v>15</v>
+      </c>
+      <c r="C442">
+        <v>25579</v>
+      </c>
+      <c r="D442">
+        <f>375/400</f>
+        <v>0.9375</v>
+      </c>
+      <c r="G442" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" ht="19">
+      <c r="A445" t="s">
+        <v>87</v>
+      </c>
+      <c r="B445" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7">
+      <c r="A446" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B446" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C446" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E446" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F446" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G446" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7">
+      <c r="A447">
+        <v>200</v>
+      </c>
+      <c r="B447">
+        <v>10</v>
+      </c>
+      <c r="C447">
+        <v>5044</v>
+      </c>
+      <c r="D447">
+        <v>0</v>
+      </c>
+      <c r="E447">
+        <v>0</v>
+      </c>
+      <c r="F447">
+        <v>1</v>
+      </c>
+      <c r="G447" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="448" spans="1:7">
+      <c r="A448">
+        <v>200</v>
+      </c>
+      <c r="B448">
+        <v>11</v>
+      </c>
+      <c r="C448">
+        <v>4803</v>
+      </c>
+      <c r="D448">
+        <v>0</v>
+      </c>
+      <c r="E448">
+        <v>0</v>
+      </c>
+      <c r="F448">
+        <v>2</v>
+      </c>
+      <c r="G448" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7">
+      <c r="A449">
+        <v>200</v>
+      </c>
+      <c r="B449">
+        <v>12</v>
+      </c>
+      <c r="C449">
+        <v>2960</v>
+      </c>
+      <c r="D449">
+        <v>0</v>
+      </c>
+      <c r="E449">
+        <v>0</v>
+      </c>
+      <c r="F449" t="s">
+        <v>171</v>
+      </c>
+      <c r="G449" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7">
+      <c r="A450">
+        <v>200</v>
+      </c>
+      <c r="B450">
+        <v>12</v>
+      </c>
+      <c r="C450">
+        <v>5622</v>
+      </c>
+      <c r="D450">
+        <v>0</v>
+      </c>
+      <c r="E450">
+        <v>0</v>
+      </c>
+      <c r="F450">
+        <v>4</v>
+      </c>
+      <c r="G450" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7">
+      <c r="A451">
+        <v>600</v>
+      </c>
+      <c r="B451">
+        <v>12</v>
+      </c>
+      <c r="C451">
+        <v>5322</v>
+      </c>
+      <c r="D451">
+        <v>0</v>
+      </c>
+      <c r="E451">
+        <v>0</v>
+      </c>
+      <c r="F451">
+        <v>5</v>
+      </c>
+      <c r="G451" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7">
+      <c r="A452">
+        <v>200</v>
+      </c>
+      <c r="B452">
+        <v>13</v>
+      </c>
+      <c r="C452">
+        <v>6071</v>
+      </c>
+      <c r="D452">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E452">
+        <f>D452*100</f>
+        <v>0.5</v>
+      </c>
+      <c r="F452">
+        <v>6</v>
+      </c>
+      <c r="G452" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7">
+      <c r="A453">
+        <v>400</v>
+      </c>
+      <c r="B453">
+        <v>13</v>
+      </c>
+      <c r="C453">
+        <v>5898</v>
+      </c>
+      <c r="D453">
+        <v>0</v>
+      </c>
+      <c r="E453">
+        <f t="shared" ref="E453:E455" si="6">D453*100</f>
+        <v>0</v>
+      </c>
+      <c r="F453">
+        <v>7</v>
+      </c>
+      <c r="G453" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7">
+      <c r="A454">
+        <v>400</v>
+      </c>
+      <c r="B454">
+        <v>14</v>
+      </c>
+      <c r="C454">
+        <v>6684</v>
+      </c>
+      <c r="D454">
+        <v>0</v>
+      </c>
+      <c r="E454">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F454">
+        <v>8</v>
+      </c>
+      <c r="G454" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7">
+      <c r="A455">
+        <v>400</v>
+      </c>
+      <c r="B455">
+        <v>15</v>
+      </c>
+      <c r="C455">
+        <v>4501</v>
+      </c>
+      <c r="D455">
+        <f>2/400</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E455">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="F455">
+        <v>9</v>
+      </c>
+      <c r="G455" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7">
+      <c r="A456">
+        <v>400</v>
+      </c>
+      <c r="B456">
+        <v>16</v>
+      </c>
+      <c r="C456">
+        <v>4934</v>
+      </c>
+      <c r="D456">
+        <v>0</v>
+      </c>
+      <c r="E456">
+        <v>0</v>
+      </c>
+      <c r="F456">
+        <v>10</v>
+      </c>
+      <c r="G456" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7">
+      <c r="A457" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7">
+      <c r="A458">
+        <v>400</v>
+      </c>
+      <c r="B458">
+        <v>17</v>
+      </c>
+      <c r="C458">
+        <v>8353</v>
+      </c>
+      <c r="D458">
+        <f>150/400</f>
+        <v>0.375</v>
+      </c>
+      <c r="E458">
+        <f>D458*100</f>
+        <v>37.5</v>
+      </c>
+      <c r="F458">
+        <v>11</v>
+      </c>
+      <c r="G458" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7">
+      <c r="A459">
+        <v>400</v>
+      </c>
+      <c r="B459">
+        <v>16</v>
+      </c>
+      <c r="C459">
+        <v>7826</v>
+      </c>
+      <c r="D459">
+        <f>242/400</f>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="E459">
+        <f>D459*100</f>
+        <v>60.5</v>
+      </c>
+      <c r="F459" t="s">
+        <v>180</v>
+      </c>
+      <c r="G459" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7">
+      <c r="A460">
+        <v>300</v>
+      </c>
+      <c r="B460">
+        <v>16</v>
+      </c>
+      <c r="C460">
+        <v>8077</v>
+      </c>
+      <c r="D460">
+        <f>212/300</f>
+        <v>0.70666666666666667</v>
+      </c>
+      <c r="E460">
+        <f>D460*100</f>
+        <v>70.666666666666671</v>
+      </c>
+      <c r="F460" t="s">
+        <v>182</v>
+      </c>
+      <c r="G460" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7">
+      <c r="A461">
+        <v>300</v>
+      </c>
+      <c r="B461">
+        <v>15</v>
+      </c>
+      <c r="C461">
+        <v>8260</v>
+      </c>
+      <c r="D461">
+        <f>187/300</f>
+        <v>0.62333333333333329</v>
+      </c>
+      <c r="E461">
+        <f>D461*100</f>
+        <v>62.333333333333329</v>
+      </c>
+      <c r="F461">
+        <v>14</v>
+      </c>
+      <c r="G461" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7">
+      <c r="A464">
+        <v>300</v>
+      </c>
+      <c r="B464">
+        <v>14</v>
+      </c>
+      <c r="C464">
+        <v>7963</v>
+      </c>
+      <c r="D464">
+        <f>62/300</f>
+        <v>0.20666666666666667</v>
+      </c>
+      <c r="E464">
+        <f>D464*100</f>
+        <v>20.666666666666668</v>
+      </c>
+      <c r="F464">
+        <v>1</v>
+      </c>
+      <c r="G464" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="465" spans="1:7">
+      <c r="A465">
+        <v>300</v>
+      </c>
+      <c r="B465">
+        <v>13</v>
+      </c>
+      <c r="C465">
+        <v>3378</v>
+      </c>
+      <c r="D465">
+        <v>0</v>
+      </c>
+      <c r="E465">
+        <f t="shared" ref="E465:E480" si="7">D465*100</f>
+        <v>0</v>
+      </c>
+      <c r="F465">
+        <v>2</v>
+      </c>
+      <c r="G465" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7">
+      <c r="A466">
+        <v>400</v>
+      </c>
+      <c r="B466">
+        <v>13</v>
+      </c>
+      <c r="C466">
+        <v>3254</v>
+      </c>
+      <c r="D466">
+        <f>1/300</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="E466">
+        <f t="shared" si="7"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="F466">
+        <v>3</v>
+      </c>
+      <c r="G466" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7">
+      <c r="A467">
+        <v>600</v>
+      </c>
+      <c r="B467">
+        <v>13</v>
+      </c>
+      <c r="C467">
+        <v>3234</v>
+      </c>
+      <c r="D467">
+        <v>0</v>
+      </c>
+      <c r="E467">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F467">
+        <v>4</v>
+      </c>
+      <c r="G467" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="468" spans="1:7">
+      <c r="A468" t="s">
+        <v>189</v>
+      </c>
+      <c r="E468">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:7">
+      <c r="A469">
+        <v>600</v>
+      </c>
+      <c r="B469">
+        <v>13</v>
+      </c>
+      <c r="C469">
+        <v>6663</v>
+      </c>
+      <c r="D469">
+        <f>1/600</f>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="E469">
+        <f t="shared" si="7"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="F469">
+        <v>5</v>
+      </c>
+      <c r="G469" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="470" spans="1:7">
+      <c r="A470">
+        <v>400</v>
+      </c>
+      <c r="B470">
+        <v>14</v>
+      </c>
+      <c r="C470">
+        <v>7267</v>
+      </c>
+      <c r="D470">
+        <f>262/400</f>
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E470">
+        <f t="shared" si="7"/>
+        <v>65.5</v>
+      </c>
+      <c r="F470" t="s">
+        <v>192</v>
+      </c>
+      <c r="G470" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="471" spans="1:7">
+      <c r="A471">
+        <v>100</v>
+      </c>
+      <c r="B471">
+        <v>20</v>
+      </c>
+      <c r="C471">
+        <v>16766</v>
+      </c>
+      <c r="D471">
+        <f>88/100</f>
+        <v>0.88</v>
+      </c>
+      <c r="E471">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="F471">
+        <v>7</v>
+      </c>
+      <c r="G471" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="472" spans="1:7">
+      <c r="A472">
+        <v>100</v>
+      </c>
+      <c r="B472">
+        <v>22</v>
+      </c>
+      <c r="C472">
+        <v>8736</v>
+      </c>
+      <c r="D472">
+        <f>80/100</f>
+        <v>0.8</v>
+      </c>
+      <c r="E472">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="F472">
+        <v>8</v>
+      </c>
+      <c r="G472" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="473" spans="1:7">
+      <c r="A473">
+        <v>100</v>
+      </c>
+      <c r="B473">
+        <v>30</v>
+      </c>
+      <c r="C473">
+        <v>7209</v>
+      </c>
+      <c r="D473">
+        <f>77/100</f>
+        <v>0.77</v>
+      </c>
+      <c r="E473">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="F473">
+        <v>9</v>
+      </c>
+      <c r="G473" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="474" spans="1:7">
+      <c r="E474">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:7">
+      <c r="A475">
+        <v>100</v>
+      </c>
+      <c r="B475">
+        <v>40</v>
+      </c>
+      <c r="C475">
+        <v>8161</v>
+      </c>
+      <c r="D475">
+        <f>77/100</f>
+        <v>0.77</v>
+      </c>
+      <c r="E475">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="F475">
+        <v>1</v>
+      </c>
+      <c r="G475" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="476" spans="1:7">
+      <c r="A476">
+        <v>100</v>
+      </c>
+      <c r="B476">
+        <v>100</v>
+      </c>
+      <c r="C476">
+        <v>14978</v>
+      </c>
+      <c r="D476">
+        <f>78/100</f>
+        <v>0.78</v>
+      </c>
+      <c r="E476">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="F476">
+        <v>2</v>
+      </c>
+      <c r="G476" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="477" spans="1:7">
+      <c r="A477">
+        <v>100</v>
+      </c>
+      <c r="B477">
+        <v>50</v>
+      </c>
+      <c r="C477">
+        <v>6741</v>
+      </c>
+      <c r="D477">
+        <f>75/100</f>
+        <v>0.75</v>
+      </c>
+      <c r="E477">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="F477">
+        <v>3</v>
+      </c>
+      <c r="G477" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="478" spans="1:7">
+      <c r="A478">
+        <v>100</v>
+      </c>
+      <c r="B478">
+        <v>13</v>
+      </c>
+      <c r="C478">
+        <v>6594</v>
+      </c>
+      <c r="D478">
+        <v>0</v>
+      </c>
+      <c r="E478">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F478">
+        <v>4</v>
+      </c>
+      <c r="G478" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="479" spans="1:7">
+      <c r="A479">
+        <v>1000</v>
+      </c>
+      <c r="B479">
+        <v>13</v>
+      </c>
+      <c r="C479">
+        <v>4980</v>
+      </c>
+      <c r="D479">
+        <f>666/1000</f>
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="E479">
+        <f t="shared" si="7"/>
+        <v>66.600000000000009</v>
+      </c>
+      <c r="F479" t="s">
+        <v>201</v>
+      </c>
+      <c r="G479" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="480" spans="1:7">
+      <c r="A480">
+        <v>60</v>
+      </c>
+      <c r="B480">
+        <v>60</v>
+      </c>
+      <c r="C480">
+        <v>5748</v>
+      </c>
+      <c r="D480">
+        <f>45/60</f>
+        <v>0.75</v>
+      </c>
+      <c r="E480">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="F480">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -30291,7 +31653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800F9AAE-03E4-C445-A42F-4AF399074101}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some changes to make new scaling MAT Pods testing work
</commit_message>
<xml_diff>
--- a/summary-info.xlsx
+++ b/summary-info.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/github/ms-fs-performance-testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B40F0F-2FB7-CC41-8FE2-1D0DA04479E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236CBE18-93A8-4244-8B55-FC9FE0AEE913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32020" yWindow="-100" windowWidth="30800" windowHeight="16000" xr2:uid="{8E989FE0-EC17-C94D-8489-988F3A88D2B8}"/>
+    <workbookView minimized="1" xWindow="52080" yWindow="7580" windowWidth="32720" windowHeight="20540" xr2:uid="{8E989FE0-EC17-C94D-8489-988F3A88D2B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26706,8 +26709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AE1DBA-CD56-294B-B978-A723FB34EE23}">
   <dimension ref="A1:H480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
-      <selection activeCell="B437" sqref="B437"/>
+    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+      <selection activeCell="G455" sqref="G455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -31650,6 +31653,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E72EAB-EF19-FC4B-9B6A-CD930ACC5DC9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800F9AAE-03E4-C445-A42F-4AF399074101}">
   <dimension ref="A1:H41"/>
   <sheetViews>
@@ -31871,7 +31888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64E26E8-C365-1E49-B425-11718AE634C5}">
   <dimension ref="A1:J31"/>
   <sheetViews>
@@ -32086,7 +32103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD05596-990E-C245-9407-CC06BFEFCD7A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
- updated the testing source code and added a few more classes - added testing scripts
</commit_message>
<xml_diff>
--- a/summary-info.xlsx
+++ b/summary-info.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/github/ms-fs-performance-testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236CBE18-93A8-4244-8B55-FC9FE0AEE913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FFA781-D93F-4042-8220-5FE3C85265FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="52080" yWindow="7580" windowWidth="32720" windowHeight="20540" xr2:uid="{8E989FE0-EC17-C94D-8489-988F3A88D2B8}"/>
+    <workbookView xWindow="19180" yWindow="760" windowWidth="39160" windowHeight="20540" activeTab="2" xr2:uid="{8E989FE0-EC17-C94D-8489-988F3A88D2B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="2019-MAT-Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="MAT-Testing" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -806,7 +804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1075,7 +1073,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$14</c:f>
+              <c:f>'2019-MAT-Testing'!$B$7:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1108,7 +1106,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$14</c:f>
+              <c:f>'2019-MAT-Testing'!$C$7:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1437,7 +1435,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$103:$B$107</c:f>
+              <c:f>'2019-MAT-Testing'!$B$103:$B$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1461,7 +1459,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$103:$C$107</c:f>
+              <c:f>'2019-MAT-Testing'!$C$103:$C$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1781,7 +1779,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$103:$G$107</c:f>
+              <c:f>'2019-MAT-Testing'!$G$103:$G$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1805,7 +1803,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$103:$H$107</c:f>
+              <c:f>'2019-MAT-Testing'!$H$103:$H$107</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2125,7 +2123,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$118:$B$122</c:f>
+              <c:f>'2019-MAT-Testing'!$B$118:$B$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2149,7 +2147,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$118:$C$122</c:f>
+              <c:f>'2019-MAT-Testing'!$C$118:$C$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2482,7 +2480,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$118:$G$122</c:f>
+              <c:f>'2019-MAT-Testing'!$G$118:$G$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2506,7 +2504,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$118:$H$122</c:f>
+              <c:f>'2019-MAT-Testing'!$H$118:$H$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2831,7 +2829,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$137:$B$140</c:f>
+              <c:f>'2019-MAT-Testing'!$B$137:$B$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2852,7 +2850,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$137:$C$140</c:f>
+              <c:f>'2019-MAT-Testing'!$C$137:$C$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3169,7 +3167,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$137:$G$140</c:f>
+              <c:f>'2019-MAT-Testing'!$G$137:$G$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3190,7 +3188,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$137:$H$140</c:f>
+              <c:f>'2019-MAT-Testing'!$H$137:$H$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3507,7 +3505,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$152:$G$155</c:f>
+              <c:f>'2019-MAT-Testing'!$G$152:$G$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3528,7 +3526,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$152:$H$155</c:f>
+              <c:f>'2019-MAT-Testing'!$H$152:$H$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3850,7 +3848,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$152:$B$155</c:f>
+              <c:f>'2019-MAT-Testing'!$B$152:$B$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3871,7 +3869,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$152:$C$155</c:f>
+              <c:f>'2019-MAT-Testing'!$C$152:$C$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4188,7 +4186,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$190:$B$202</c:f>
+              <c:f>'2019-MAT-Testing'!$B$190:$B$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4236,7 +4234,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$190:$C$202</c:f>
+              <c:f>'2019-MAT-Testing'!$C$190:$C$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4580,7 +4578,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$190:$G$202</c:f>
+              <c:f>'2019-MAT-Testing'!$G$190:$G$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4628,7 +4626,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$190:$H$202</c:f>
+              <c:f>'2019-MAT-Testing'!$H$190:$H$202</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4977,7 +4975,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$B$27</c:f>
+              <c:f>'2019-MAT-Testing'!$B$24:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4998,7 +4996,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$24:$C$27</c:f>
+              <c:f>'2019-MAT-Testing'!$C$24:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5315,7 +5313,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$209:$B$214</c:f>
+              <c:f>'2019-MAT-Testing'!$B$209:$B$214</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5342,7 +5340,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$209:$C$214</c:f>
+              <c:f>'2019-MAT-Testing'!$C$209:$C$214</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5665,7 +5663,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$209:$G$214</c:f>
+              <c:f>'2019-MAT-Testing'!$G$209:$G$214</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5692,7 +5690,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$209:$H$214</c:f>
+              <c:f>'2019-MAT-Testing'!$H$209:$H$214</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6015,7 +6013,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$228:$B$230</c:f>
+              <c:f>'2019-MAT-Testing'!$B$228:$B$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6033,7 +6031,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$228:$C$230</c:f>
+              <c:f>'2019-MAT-Testing'!$C$228:$C$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6347,7 +6345,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$228:$G$230</c:f>
+              <c:f>'2019-MAT-Testing'!$G$228:$G$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6365,7 +6363,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$228:$H$230</c:f>
+              <c:f>'2019-MAT-Testing'!$H$228:$H$230</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6691,7 +6689,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$242:$G$248</c:f>
+              <c:f>'2019-MAT-Testing'!$G$242:$G$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6721,7 +6719,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$242:$H$248</c:f>
+              <c:f>'2019-MAT-Testing'!$H$242:$H$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7052,7 +7050,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$242:$B$248</c:f>
+              <c:f>'2019-MAT-Testing'!$B$242:$B$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7082,7 +7080,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$242:$C$248</c:f>
+              <c:f>'2019-MAT-Testing'!$C$242:$C$248</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7413,7 +7411,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$260:$G$264</c:f>
+              <c:f>'2019-MAT-Testing'!$G$260:$G$264</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7437,7 +7435,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$260:$H$264</c:f>
+              <c:f>'2019-MAT-Testing'!$H$260:$H$264</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7762,7 +7760,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$275:$G$281</c:f>
+              <c:f>'2019-MAT-Testing'!$G$275:$G$281</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7792,7 +7790,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$275:$H$281</c:f>
+              <c:f>'2019-MAT-Testing'!$H$275:$H$281</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -8118,7 +8116,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$24:$G$27</c:f>
+              <c:f>'2019-MAT-Testing'!$G$24:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8139,7 +8137,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$24:$H$27</c:f>
+              <c:f>'2019-MAT-Testing'!$H$24:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8456,7 +8454,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$55:$B$58</c:f>
+              <c:f>'2019-MAT-Testing'!$B$55:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8477,7 +8475,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$55:$C$58</c:f>
+              <c:f>'2019-MAT-Testing'!$C$55:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8794,7 +8792,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$55:$G$58</c:f>
+              <c:f>'2019-MAT-Testing'!$G$55:$G$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8815,7 +8813,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$55:$H$58</c:f>
+              <c:f>'2019-MAT-Testing'!$H$55:$H$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9132,7 +9130,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$70:$B$73</c:f>
+              <c:f>'2019-MAT-Testing'!$B$70:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9153,7 +9151,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$70:$C$73</c:f>
+              <c:f>'2019-MAT-Testing'!$C$70:$C$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9470,7 +9468,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$70:$G$73</c:f>
+              <c:f>'2019-MAT-Testing'!$G$70:$G$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9491,7 +9489,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$70:$H$73</c:f>
+              <c:f>'2019-MAT-Testing'!$H$70:$H$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9813,7 +9811,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$88:$B$94</c:f>
+              <c:f>'2019-MAT-Testing'!$B$88:$B$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -9843,7 +9841,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$88:$C$94</c:f>
+              <c:f>'2019-MAT-Testing'!$C$88:$C$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -10169,7 +10167,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$88:$G$94</c:f>
+              <c:f>'2019-MAT-Testing'!$G$88:$G$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -10199,7 +10197,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$88:$H$94</c:f>
+              <c:f>'2019-MAT-Testing'!$H$88:$H$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -26709,11 +26707,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AE1DBA-CD56-294B-B978-A723FB34EE23}">
   <dimension ref="A1:H480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+    <sheetView topLeftCell="A256" workbookViewId="0">
       <selection activeCell="G455" sqref="G455"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="34.5" customWidth="1"/>
@@ -26725,17 +26723,17 @@
     <col min="11" max="11" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="21">
+    <row r="1" spans="2:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
@@ -26743,7 +26741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -26754,7 +26752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>10</v>
       </c>
@@ -26765,7 +26763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>20</v>
       </c>
@@ -26776,7 +26774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>30</v>
       </c>
@@ -26787,7 +26785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>40</v>
       </c>
@@ -26798,7 +26796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>50</v>
       </c>
@@ -26809,7 +26807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>60</v>
       </c>
@@ -26820,7 +26818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>80</v>
       </c>
@@ -26831,7 +26829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>100</v>
       </c>
@@ -26839,7 +26837,7 @@
         <v>21433</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
@@ -26847,7 +26845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -26855,7 +26853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -26866,7 +26864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>10</v>
       </c>
@@ -26883,7 +26881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>15</v>
       </c>
@@ -26901,7 +26899,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>20</v>
       </c>
@@ -26919,7 +26917,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>30</v>
       </c>
@@ -26937,7 +26935,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
@@ -26945,12 +26943,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>26</v>
       </c>
@@ -26958,7 +26956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>25</v>
       </c>
@@ -26969,7 +26967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>27</v>
       </c>
@@ -26980,7 +26978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>28</v>
       </c>
@@ -26991,7 +26989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>29</v>
       </c>
@@ -27002,7 +27000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>30</v>
       </c>
@@ -27013,7 +27011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>31</v>
       </c>
@@ -27024,7 +27022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>32</v>
       </c>
@@ -27035,18 +27033,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="2:8">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
     </row>
-    <row r="51" spans="2:8">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>15</v>
       </c>
@@ -27054,12 +27052,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="2:8">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>11</v>
       </c>
@@ -27067,7 +27065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="2:8">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>18</v>
       </c>
@@ -27078,7 +27076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="2:8">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>10</v>
       </c>
@@ -27096,7 +27094,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="56" spans="2:8">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>15</v>
       </c>
@@ -27114,7 +27112,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="57" spans="2:8">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>20</v>
       </c>
@@ -27132,7 +27130,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="58" spans="2:8">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>25</v>
       </c>
@@ -27150,12 +27148,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="59" spans="2:8">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="2:8">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
         <v>12</v>
       </c>
@@ -27163,7 +27161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="2:8">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>10</v>
       </c>
@@ -27181,7 +27179,7 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="71" spans="2:8">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>15</v>
       </c>
@@ -27199,7 +27197,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="72" spans="2:8">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>20</v>
       </c>
@@ -27217,7 +27215,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="73" spans="2:8">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>25</v>
       </c>
@@ -27235,17 +27233,17 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="74" spans="2:8">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="2:8">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="2:8">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B86" s="2" t="s">
         <v>23</v>
       </c>
@@ -27253,7 +27251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="2:8">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>36</v>
       </c>
@@ -27264,7 +27262,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="2:8">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B88">
         <v>10</v>
       </c>
@@ -27282,7 +27280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>20</v>
       </c>
@@ -27300,7 +27298,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="90" spans="2:8">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B90">
         <v>25</v>
       </c>
@@ -27317,7 +27315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:8">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B91">
         <v>30</v>
       </c>
@@ -27334,7 +27332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B92">
         <v>40</v>
       </c>
@@ -27352,7 +27350,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="93" spans="2:8">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B93">
         <v>45</v>
       </c>
@@ -27370,7 +27368,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="94" spans="2:8">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B94">
         <v>50</v>
       </c>
@@ -27388,7 +27386,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="100" spans="2:8">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100" s="2" t="s">
         <v>23</v>
       </c>
@@ -27396,7 +27394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="2:8">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>37</v>
       </c>
@@ -27404,12 +27402,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="102" spans="2:8">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B102" s="4">
         <v>43762</v>
       </c>
     </row>
-    <row r="103" spans="2:8">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B103">
         <v>30</v>
       </c>
@@ -27426,7 +27424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B104">
         <v>40</v>
       </c>
@@ -27444,7 +27442,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="105" spans="2:8">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B105">
         <v>45</v>
       </c>
@@ -27462,7 +27460,7 @@
         <v>0.24444444444444444</v>
       </c>
     </row>
-    <row r="106" spans="2:8">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B106">
         <v>50</v>
       </c>
@@ -27480,7 +27478,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="107" spans="2:8">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B107">
         <v>60</v>
       </c>
@@ -27498,12 +27496,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="117" spans="2:8">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B117" s="4">
         <v>43763</v>
       </c>
     </row>
-    <row r="118" spans="2:8">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B118">
         <v>20</v>
       </c>
@@ -27520,7 +27518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B119">
         <v>30</v>
       </c>
@@ -27538,7 +27536,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="120" spans="2:8">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B120">
         <v>40</v>
       </c>
@@ -27556,7 +27554,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="121" spans="2:8">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B121">
         <v>50</v>
       </c>
@@ -27574,7 +27572,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="122" spans="2:8">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B122">
         <v>60</v>
       </c>
@@ -27592,12 +27590,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="134" spans="2:8" ht="21">
+    <row r="134" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B134" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="135" spans="2:8">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" s="2" t="s">
         <v>49</v>
       </c>
@@ -27605,7 +27603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="136" spans="2:8">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>50</v>
       </c>
@@ -27616,7 +27614,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="137" spans="2:8">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137">
         <v>10</v>
       </c>
@@ -27633,7 +27631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:8">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B138">
         <v>20</v>
       </c>
@@ -27650,7 +27648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="2:8">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B139">
         <v>25</v>
       </c>
@@ -27668,7 +27666,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="140" spans="2:8">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B140">
         <v>30</v>
       </c>
@@ -27686,12 +27684,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="151" spans="2:8">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C151" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="152" spans="2:8">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B152">
         <v>10</v>
       </c>
@@ -27708,7 +27706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:8">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B153">
         <v>20</v>
       </c>
@@ -27725,7 +27723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:8">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B154">
         <v>25</v>
       </c>
@@ -27743,7 +27741,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="155" spans="2:8">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B155">
         <v>30</v>
       </c>
@@ -27761,12 +27759,12 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="167" spans="2:7" ht="21">
+    <row r="167" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B167" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="168" spans="2:7">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B168" s="6" t="s">
         <v>59</v>
       </c>
@@ -27779,7 +27777,7 @@
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
     </row>
-    <row r="169" spans="2:7">
+    <row r="169" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B169" s="6" t="s">
         <v>58</v>
       </c>
@@ -27792,7 +27790,7 @@
       <c r="E169" s="6"/>
       <c r="F169" s="6"/>
     </row>
-    <row r="170" spans="2:7">
+    <row r="170" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B170" s="6" t="s">
         <v>60</v>
       </c>
@@ -27805,12 +27803,12 @@
       <c r="E170" s="6"/>
       <c r="F170" s="6"/>
     </row>
-    <row r="174" spans="2:7">
+    <row r="174" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B174" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="176" spans="2:7">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B176">
         <v>20</v>
       </c>
@@ -27824,7 +27822,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="177" spans="2:8">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B177">
         <v>25</v>
       </c>
@@ -27835,7 +27833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="2:8">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B178">
         <v>30</v>
       </c>
@@ -27846,7 +27844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="2:8">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B179">
         <v>35</v>
       </c>
@@ -27857,7 +27855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="2:8">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B180">
         <v>40</v>
       </c>
@@ -27868,7 +27866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="2:8">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>56</v>
       </c>
@@ -27879,7 +27877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="2:8">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>57</v>
       </c>
@@ -27890,17 +27888,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="185" spans="2:8">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B185" s="4">
         <v>43767</v>
       </c>
     </row>
-    <row r="188" spans="2:8" ht="21">
+    <row r="188" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B188" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="189" spans="2:8">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B189" s="2" t="s">
         <v>61</v>
       </c>
@@ -27911,7 +27909,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="190" spans="2:8">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B190">
         <v>20</v>
       </c>
@@ -27928,7 +27926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="2:8">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B191">
         <v>25</v>
       </c>
@@ -27945,7 +27943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="2:8">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B192">
         <v>30</v>
       </c>
@@ -27962,7 +27960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="2:8">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B193">
         <v>40</v>
       </c>
@@ -27979,7 +27977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="2:8">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B194">
         <v>50</v>
       </c>
@@ -27996,7 +27994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="2:8">
+    <row r="195" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B195">
         <v>60</v>
       </c>
@@ -28015,7 +28013,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="196" spans="2:8">
+    <row r="196" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B196">
         <v>65</v>
       </c>
@@ -28032,7 +28030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="2:8">
+    <row r="197" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B197">
         <v>70</v>
       </c>
@@ -28049,7 +28047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="2:8">
+    <row r="198" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B198">
         <v>80</v>
       </c>
@@ -28068,7 +28066,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="199" spans="2:8">
+    <row r="199" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B199">
         <v>90</v>
       </c>
@@ -28087,7 +28085,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="200" spans="2:8">
+    <row r="200" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B200">
         <v>100</v>
       </c>
@@ -28106,7 +28104,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="201" spans="2:8">
+    <row r="201" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B201">
         <v>110</v>
       </c>
@@ -28125,7 +28123,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="202" spans="2:8">
+    <row r="202" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B202">
         <v>120</v>
       </c>
@@ -28144,17 +28142,17 @@
         <v>0.16166666666666665</v>
       </c>
     </row>
-    <row r="204" spans="2:8">
+    <row r="204" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B204" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="207" spans="2:8" ht="21">
+    <row r="207" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B207" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="208" spans="2:8">
+    <row r="208" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B208" s="2" t="s">
         <v>61</v>
       </c>
@@ -28162,7 +28160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="209" spans="2:8">
+    <row r="209" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B209">
         <v>20</v>
       </c>
@@ -28179,7 +28177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="2:8">
+    <row r="210" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B210">
         <v>25</v>
       </c>
@@ -28196,7 +28194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="2:8">
+    <row r="211" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B211">
         <v>30</v>
       </c>
@@ -28213,7 +28211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="2:8">
+    <row r="212" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B212">
         <v>40</v>
       </c>
@@ -28230,7 +28228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="2:8">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B213">
         <v>50</v>
       </c>
@@ -28247,7 +28245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="2:8">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B214">
         <v>60</v>
       </c>
@@ -28266,17 +28264,17 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="216" spans="2:8">
+    <row r="216" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B216" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="225" spans="2:8" ht="21">
+    <row r="225" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B225" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="226" spans="2:8">
+    <row r="226" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B226" s="2" t="s">
         <v>61</v>
       </c>
@@ -28287,12 +28285,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="227" spans="2:8">
+    <row r="227" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B227">
         <v>20</v>
       </c>
     </row>
-    <row r="228" spans="2:8">
+    <row r="228" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B228">
         <v>24</v>
       </c>
@@ -28309,7 +28307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="2:8">
+    <row r="229" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B229">
         <v>30</v>
       </c>
@@ -28328,7 +28326,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="230" spans="2:8">
+    <row r="230" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B230">
         <v>40</v>
       </c>
@@ -28347,12 +28345,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="240" spans="2:8" ht="21">
+    <row r="240" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B240" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="241" spans="2:8">
+    <row r="241" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B241" s="2" t="s">
         <v>61</v>
       </c>
@@ -28363,7 +28361,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="242" spans="2:8">
+    <row r="242" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B242">
         <v>20</v>
       </c>
@@ -28380,7 +28378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="2:8">
+    <row r="243" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B243">
         <v>25</v>
       </c>
@@ -28399,7 +28397,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="244" spans="2:8">
+    <row r="244" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B244">
         <v>30</v>
       </c>
@@ -28416,7 +28414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="2:8">
+    <row r="245" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B245">
         <v>35</v>
       </c>
@@ -28433,7 +28431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="2:8">
+    <row r="246" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B246">
         <v>40</v>
       </c>
@@ -28452,7 +28450,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="247" spans="2:8">
+    <row r="247" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B247">
         <v>45</v>
       </c>
@@ -28471,7 +28469,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="248" spans="2:8">
+    <row r="248" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B248">
         <v>50</v>
       </c>
@@ -28490,17 +28488,17 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="4">
         <v>43773</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="19">
+    <row r="258" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B258" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
         <v>70</v>
       </c>
@@ -28518,7 +28516,7 @@
       </c>
       <c r="F259" s="2"/>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1000</v>
       </c>
@@ -28544,7 +28542,7 @@
         <v>1.0999999999999999</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>200</v>
       </c>
@@ -28569,7 +28567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>200</v>
       </c>
@@ -28595,7 +28593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>200</v>
       </c>
@@ -28621,7 +28619,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>200</v>
       </c>
@@ -28647,12 +28645,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="19">
+    <row r="274" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B274" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>200</v>
       </c>
@@ -28677,7 +28675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>600</v>
       </c>
@@ -28701,7 +28699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1000</v>
       </c>
@@ -28726,7 +28724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>200</v>
       </c>
@@ -28751,7 +28749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>600</v>
       </c>
@@ -28777,7 +28775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>200</v>
       </c>
@@ -28803,7 +28801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>200</v>
       </c>
@@ -28829,7 +28827,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="19">
+    <row r="290" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A290" s="4">
         <v>43775</v>
       </c>
@@ -28837,13 +28835,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="291" spans="1:6" ht="19">
+    <row r="291" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B291" s="13"/>
     </row>
-    <row r="292" spans="1:6">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292" s="2" t="s">
         <v>70</v>
       </c>
@@ -28861,7 +28859,7 @@
       </c>
       <c r="F292" s="2"/>
     </row>
-    <row r="293" spans="1:6">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293" s="12">
         <v>200</v>
       </c>
@@ -28875,7 +28873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:6">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" s="12">
         <v>200</v>
       </c>
@@ -28889,7 +28887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:6">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295" s="12">
         <v>200</v>
       </c>
@@ -28903,7 +28901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:6">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296" s="12">
         <v>200</v>
       </c>
@@ -28917,7 +28915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:6">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" s="12">
         <v>200</v>
       </c>
@@ -28931,7 +28929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:6">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" s="12">
         <v>200</v>
       </c>
@@ -28945,7 +28943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:6">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" s="12">
         <v>200</v>
       </c>
@@ -28959,7 +28957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:6">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300" s="12">
         <v>200</v>
       </c>
@@ -28973,7 +28971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:6">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" s="12">
         <v>200</v>
       </c>
@@ -28987,18 +28985,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:6">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302" s="12"/>
     </row>
-    <row r="303" spans="1:6">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" s="12"/>
     </row>
-    <row r="304" spans="1:6">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="305" spans="1:4">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>200</v>
       </c>
@@ -29012,7 +29010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:4">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>200</v>
       </c>
@@ -29026,7 +29024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>200</v>
       </c>
@@ -29040,7 +29038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:4">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>200</v>
       </c>
@@ -29054,7 +29052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:4">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>200</v>
       </c>
@@ -29068,7 +29066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>200</v>
       </c>
@@ -29082,7 +29080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:4">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>200</v>
       </c>
@@ -29096,7 +29094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:4">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>200</v>
       </c>
@@ -29110,7 +29108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:4">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>260</v>
       </c>
@@ -29124,7 +29122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>280</v>
       </c>
@@ -29138,7 +29136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:4">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>300</v>
       </c>
@@ -29152,7 +29150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:4">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>300</v>
       </c>
@@ -29166,7 +29164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:4">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>320</v>
       </c>
@@ -29180,12 +29178,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="19">
+    <row r="320" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B320" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="321" spans="1:6">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" s="2" t="s">
         <v>70</v>
       </c>
@@ -29203,7 +29201,7 @@
       </c>
       <c r="F321" s="2"/>
     </row>
-    <row r="322" spans="1:6">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" s="12">
         <v>200</v>
       </c>
@@ -29222,7 +29220,7 @@
       </c>
       <c r="F322" s="12"/>
     </row>
-    <row r="323" spans="1:6">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" s="12">
         <v>200</v>
       </c>
@@ -29241,7 +29239,7 @@
       </c>
       <c r="F323" s="12"/>
     </row>
-    <row r="324" spans="1:6">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" s="12">
         <v>200</v>
       </c>
@@ -29260,7 +29258,7 @@
       </c>
       <c r="F324" s="12"/>
     </row>
-    <row r="325" spans="1:6">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" s="12">
         <v>200</v>
       </c>
@@ -29279,7 +29277,7 @@
       </c>
       <c r="F325" s="12"/>
     </row>
-    <row r="326" spans="1:6">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>200</v>
       </c>
@@ -29299,7 +29297,7 @@
       </c>
       <c r="F326" s="12"/>
     </row>
-    <row r="327" spans="1:6">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>200</v>
       </c>
@@ -29319,7 +29317,7 @@
       </c>
       <c r="F327" s="12"/>
     </row>
-    <row r="328" spans="1:6">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>200</v>
       </c>
@@ -29339,7 +29337,7 @@
       </c>
       <c r="F328" s="12"/>
     </row>
-    <row r="329" spans="1:6">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>200</v>
       </c>
@@ -29359,7 +29357,7 @@
       </c>
       <c r="F329" s="12"/>
     </row>
-    <row r="330" spans="1:6">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>200</v>
       </c>
@@ -29379,7 +29377,7 @@
       </c>
       <c r="F330" s="12"/>
     </row>
-    <row r="331" spans="1:6">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>200</v>
       </c>
@@ -29399,7 +29397,7 @@
       </c>
       <c r="F331" s="12"/>
     </row>
-    <row r="332" spans="1:6">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>200</v>
       </c>
@@ -29419,17 +29417,17 @@
       </c>
       <c r="F332" s="12"/>
     </row>
-    <row r="335" spans="1:6">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A335" s="4">
         <v>43776</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="153">
+    <row r="336" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="B336" s="14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="337" spans="1:7" ht="19">
+    <row r="337" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>80</v>
       </c>
@@ -29437,7 +29435,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" s="2" t="s">
         <v>70</v>
       </c>
@@ -29460,7 +29458,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>200</v>
       </c>
@@ -29482,7 +29480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>200</v>
       </c>
@@ -29503,7 +29501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>200</v>
       </c>
@@ -29523,7 +29521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>200</v>
       </c>
@@ -29544,7 +29542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>200</v>
       </c>
@@ -29566,7 +29564,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>200</v>
       </c>
@@ -29588,7 +29586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>200</v>
       </c>
@@ -29610,7 +29608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>200</v>
       </c>
@@ -29635,7 +29633,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>200</v>
       </c>
@@ -29660,12 +29658,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="353" spans="1:7">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>200</v>
       </c>
@@ -29685,7 +29683,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>200</v>
       </c>
@@ -29702,7 +29700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>200</v>
       </c>
@@ -29719,7 +29717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:7">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>200</v>
       </c>
@@ -29736,7 +29734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>200</v>
       </c>
@@ -29753,7 +29751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>200</v>
       </c>
@@ -29770,7 +29768,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="362" spans="1:7" ht="19">
+    <row r="362" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>87</v>
       </c>
@@ -29778,7 +29776,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A363" s="2" t="s">
         <v>70</v>
       </c>
@@ -29801,7 +29799,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>200</v>
       </c>
@@ -29821,7 +29819,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>200</v>
       </c>
@@ -29841,7 +29839,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>200</v>
       </c>
@@ -29861,7 +29859,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>200</v>
       </c>
@@ -29881,7 +29879,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>200</v>
       </c>
@@ -29901,7 +29899,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="369" spans="1:7">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>200</v>
       </c>
@@ -29921,7 +29919,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="370" spans="1:7">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>300</v>
       </c>
@@ -29941,7 +29939,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>600</v>
       </c>
@@ -29961,7 +29959,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="372" spans="1:7">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>1000</v>
       </c>
@@ -29984,7 +29982,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="373" spans="1:7">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>200</v>
       </c>
@@ -30005,12 +30003,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="376" spans="1:7">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="377" spans="1:7">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>200</v>
       </c>
@@ -30030,7 +30028,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="378" spans="1:7">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>200</v>
       </c>
@@ -30050,7 +30048,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="379" spans="1:7">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>200</v>
       </c>
@@ -30070,7 +30068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="380" spans="1:7">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>200</v>
       </c>
@@ -30090,7 +30088,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="381" spans="1:7">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>600</v>
       </c>
@@ -30110,7 +30108,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="382" spans="1:7" ht="409.6">
+    <row r="382" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>200</v>
       </c>
@@ -30134,7 +30132,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="383" spans="1:7">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>200</v>
       </c>
@@ -30158,7 +30156,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="384" spans="1:7">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>200</v>
       </c>
@@ -30182,7 +30180,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="385" spans="1:7">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>31</v>
       </c>
@@ -30202,7 +30200,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="386" spans="1:7">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>62</v>
       </c>
@@ -30219,7 +30217,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="387" spans="1:7">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>124</v>
       </c>
@@ -30236,7 +30234,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="388" spans="1:7">
+    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>155</v>
       </c>
@@ -30260,17 +30258,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="391" spans="1:7">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A391" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="392" spans="1:7">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="393" spans="1:7" ht="19">
+    <row r="393" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>80</v>
       </c>
@@ -30281,7 +30279,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="394" spans="1:7">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A394" s="2" t="s">
         <v>70</v>
       </c>
@@ -30301,7 +30299,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="395" spans="1:7">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>200</v>
       </c>
@@ -30322,7 +30320,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="396" spans="1:7">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>200</v>
       </c>
@@ -30339,7 +30337,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="397" spans="1:7">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>200</v>
       </c>
@@ -30356,7 +30354,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="398" spans="1:7">
+    <row r="398" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>200</v>
       </c>
@@ -30374,7 +30372,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="399" spans="1:7">
+    <row r="399" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>200</v>
       </c>
@@ -30392,7 +30390,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="400" spans="1:7">
+    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>200</v>
       </c>
@@ -30410,7 +30408,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="404" spans="1:7" ht="19">
+    <row r="404" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>131</v>
       </c>
@@ -30421,7 +30419,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="405" spans="1:7">
+    <row r="405" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A405" s="2" t="s">
         <v>70</v>
       </c>
@@ -30441,7 +30439,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="406" spans="1:7">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>200</v>
       </c>
@@ -30461,7 +30459,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="407" spans="1:7">
+    <row r="407" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>200</v>
       </c>
@@ -30481,7 +30479,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="408" spans="1:7">
+    <row r="408" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>200</v>
       </c>
@@ -30501,7 +30499,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="409" spans="1:7">
+    <row r="409" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>200</v>
       </c>
@@ -30525,12 +30523,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="411" spans="1:7">
+    <row r="411" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C411" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="412" spans="1:7">
+    <row r="412" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>200</v>
       </c>
@@ -30547,7 +30545,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="413" spans="1:7">
+    <row r="413" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>200</v>
       </c>
@@ -30568,7 +30566,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="414" spans="1:7">
+    <row r="414" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>200</v>
       </c>
@@ -30585,7 +30583,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="415" spans="1:7">
+    <row r="415" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>200</v>
       </c>
@@ -30606,7 +30604,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="419" spans="1:7" ht="19">
+    <row r="419" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A419" s="17">
         <v>43782</v>
       </c>
@@ -30614,52 +30612,52 @@
         <v>143</v>
       </c>
     </row>
-    <row r="420" spans="1:7">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B420" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="421" spans="1:7">
+    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B421" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="422" spans="1:7">
+    <row r="422" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B422" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B423" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="424" spans="1:7">
+    <row r="424" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B424" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="425" spans="1:7">
+    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B425" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="426" spans="1:7">
+    <row r="426" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B426" s="15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="427" spans="1:7">
+    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B427" s="15" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="428" spans="1:7">
+    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>200</v>
       </c>
@@ -30676,7 +30674,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="430" spans="1:7">
+    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>200</v>
       </c>
@@ -30693,7 +30691,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="431" spans="1:7">
+    <row r="431" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>400</v>
       </c>
@@ -30710,7 +30708,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="432" spans="1:7">
+    <row r="432" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>200</v>
       </c>
@@ -30727,7 +30725,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="433" spans="1:7">
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>400</v>
       </c>
@@ -30744,7 +30742,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="434" spans="1:7">
+    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>600</v>
       </c>
@@ -30761,7 +30759,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="435" spans="1:7">
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>200</v>
       </c>
@@ -30779,7 +30777,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="436" spans="1:7">
+    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>400</v>
       </c>
@@ -30797,7 +30795,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="437" spans="1:7">
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>600</v>
       </c>
@@ -30815,12 +30813,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="438" spans="1:7">
+    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="439" spans="1:7">
+    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>800</v>
       </c>
@@ -30837,7 +30835,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="440" spans="1:7">
+    <row r="440" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>200</v>
       </c>
@@ -30854,7 +30852,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="441" spans="1:7">
+    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>200</v>
       </c>
@@ -30872,7 +30870,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="442" spans="1:7">
+    <row r="442" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>400</v>
       </c>
@@ -30890,7 +30888,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="445" spans="1:7" ht="19">
+    <row r="445" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>87</v>
       </c>
@@ -30898,7 +30896,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="446" spans="1:7">
+    <row r="446" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A446" s="2" t="s">
         <v>70</v>
       </c>
@@ -30921,7 +30919,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="447" spans="1:7">
+    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>200</v>
       </c>
@@ -30944,7 +30942,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="448" spans="1:7">
+    <row r="448" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>200</v>
       </c>
@@ -30967,7 +30965,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="449" spans="1:7">
+    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>200</v>
       </c>
@@ -30990,7 +30988,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="450" spans="1:7">
+    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>200</v>
       </c>
@@ -31013,7 +31011,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="451" spans="1:7">
+    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>600</v>
       </c>
@@ -31036,7 +31034,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="452" spans="1:7">
+    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>200</v>
       </c>
@@ -31061,7 +31059,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="453" spans="1:7">
+    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>400</v>
       </c>
@@ -31085,7 +31083,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="454" spans="1:7">
+    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>400</v>
       </c>
@@ -31109,7 +31107,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="455" spans="1:7">
+    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>400</v>
       </c>
@@ -31134,7 +31132,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="456" spans="1:7">
+    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>400</v>
       </c>
@@ -31157,12 +31155,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="457" spans="1:7">
+    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="458" spans="1:7">
+    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>400</v>
       </c>
@@ -31187,7 +31185,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>400</v>
       </c>
@@ -31212,7 +31210,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="460" spans="1:7">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>300</v>
       </c>
@@ -31237,7 +31235,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="461" spans="1:7">
+    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>300</v>
       </c>
@@ -31262,7 +31260,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="464" spans="1:7">
+    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>300</v>
       </c>
@@ -31287,7 +31285,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="465" spans="1:7">
+    <row r="465" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>300</v>
       </c>
@@ -31311,7 +31309,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="466" spans="1:7">
+    <row r="466" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>400</v>
       </c>
@@ -31336,7 +31334,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="467" spans="1:7">
+    <row r="467" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>600</v>
       </c>
@@ -31360,7 +31358,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="468" spans="1:7">
+    <row r="468" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>189</v>
       </c>
@@ -31369,7 +31367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:7">
+    <row r="469" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A469">
         <v>600</v>
       </c>
@@ -31394,7 +31392,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="470" spans="1:7">
+    <row r="470" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>400</v>
       </c>
@@ -31419,7 +31417,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="471" spans="1:7">
+    <row r="471" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A471">
         <v>100</v>
       </c>
@@ -31444,7 +31442,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="472" spans="1:7">
+    <row r="472" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A472">
         <v>100</v>
       </c>
@@ -31469,7 +31467,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="473" spans="1:7">
+    <row r="473" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A473">
         <v>100</v>
       </c>
@@ -31494,13 +31492,13 @@
         <v>195</v>
       </c>
     </row>
-    <row r="474" spans="1:7">
+    <row r="474" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E474">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:7">
+    <row r="475" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A475">
         <v>100</v>
       </c>
@@ -31525,7 +31523,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="476" spans="1:7">
+    <row r="476" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A476">
         <v>100</v>
       </c>
@@ -31550,7 +31548,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="477" spans="1:7">
+    <row r="477" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A477">
         <v>100</v>
       </c>
@@ -31575,7 +31573,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="478" spans="1:7">
+    <row r="478" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A478">
         <v>100</v>
       </c>
@@ -31599,7 +31597,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="479" spans="1:7">
+    <row r="479" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A479">
         <v>1000</v>
       </c>
@@ -31624,7 +31622,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="480" spans="1:7">
+    <row r="480" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A480">
         <v>60</v>
       </c>
@@ -31653,242 +31651,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E72EAB-EF19-FC4B-9B6A-CD930ACC5DC9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800F9AAE-03E4-C445-A42F-4AF399074101}">
-  <dimension ref="A1:H41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1">
-        <v>199</v>
-      </c>
-      <c r="H1">
-        <f>12500*12</f>
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>3925</v>
-      </c>
-      <c r="B2">
-        <v>3925</v>
-      </c>
-      <c r="H2">
-        <f>H1 - (1900 + 2850)*12</f>
-        <v>93000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>2599.84</v>
-      </c>
-      <c r="B3">
-        <v>2599.84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>407.41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>210.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>202.33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
-        <v>26.88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>364.52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <v>4436.95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <v>128.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
-        <v>171.66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16">
-        <v>136.88999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>109.79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>37.270000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="B19">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <f>SUM(A1:A18)</f>
-        <v>13494.600000000002</v>
-      </c>
-      <c r="B22">
-        <f>SUM(B1:B19)</f>
-        <v>8524.84</v>
-      </c>
-      <c r="C22">
-        <f>A22-B22</f>
-        <v>4969.760000000002</v>
-      </c>
-      <c r="D22">
-        <f>(C22+1000)*12</f>
-        <v>71637.120000000024</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <v>3925</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
-        <v>2556.34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
-        <v>407.41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
-        <v>210.56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>127.23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>2416.38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>1905.77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
-        <v>95.37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
-        <v>129.77000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34">
-        <v>95.37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35">
-        <v>176.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37">
-        <v>171.66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41">
-        <f>SUM(A25:A38)</f>
-        <v>12292.260000000002</v>
-      </c>
-      <c r="B41">
-        <f>A41-A25-A26</f>
-        <v>5810.9200000000019</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64E26E8-C365-1E49-B425-11718AE634C5}">
   <dimension ref="A1:J31"/>
   <sheetViews>
@@ -31896,55 +31658,55 @@
       <selection activeCell="C25" sqref="C25:K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="3:10">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>2</v>
       </c>
@@ -31970,7 +31732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="3:10">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C26">
         <v>206</v>
       </c>
@@ -31990,7 +31752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:10">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>406</v>
       </c>
@@ -32010,7 +31772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:10">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C28">
         <v>606</v>
       </c>
@@ -32030,7 +31792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:10">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C29">
         <v>806</v>
       </c>
@@ -32051,7 +31813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:10">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C30">
         <v>1006</v>
       </c>
@@ -32072,7 +31834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:10">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C31">
         <v>1403</v>
       </c>
@@ -32103,18 +31865,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD05596-990E-C245-9407-CC06BFEFCD7A}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800F9AAE-03E4-C445-A42F-4AF399074101}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="A213" sqref="A213"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>